<commit_message>
add fun for save data and change method in bst
</commit_message>
<xml_diff>
--- a/test_data/A.xlsx
+++ b/test_data/A.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Павелецкая</t>
   </si>
@@ -29,7 +29,7 @@
 37.63612</t>
   </si>
   <si>
-    <t xml:space="preserve">Новокузнецкая</t>
+    <t xml:space="preserve">Новокосино</t>
   </si>
   <si>
     <t xml:space="preserve">55.740539, 
@@ -55,6 +55,13 @@
   <si>
     <t xml:space="preserve">55.72658,
  37.62462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Новокузнецкая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55.74212,
+37.62901</t>
   </si>
 </sst>
 </file>
@@ -69,6 +76,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,13 +162,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
@@ -204,6 +212,14 @@
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>